<commit_message>
update testing module & apis for translatros; update setup.py for installation
</commit_message>
<xml_diff>
--- a/translators/STRING/protList_STRING_interactions.xlsx
+++ b/translators/STRING/protList_STRING_interactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9606.ENSP00000495360</t>
+          <t>9606.ENSP00000269305</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CTNNB1</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.901</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -596,16 +596,16 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.049</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.13</v>
+        <v>0.292</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="4">
@@ -619,7 +619,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9606.ENSP00000269305</t>
+          <t>9606.ENSP00000419060</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>BRAF</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.947</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -650,16 +650,16 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.128</v>
       </c>
       <c r="L4" t="n">
-        <v>0.292</v>
+        <v>0.19</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.92</v>
+        <v>0.931</v>
       </c>
     </row>
     <row r="5">
@@ -673,7 +673,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>9606.ENSP00000269305</t>
+          <t>9606.ENSP00000361021</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>PTEN</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -704,16 +704,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.112</v>
       </c>
       <c r="L5" t="n">
-        <v>0.292</v>
+        <v>0.134</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N5" t="n">
-        <v>0.92</v>
+        <v>0.949</v>
       </c>
     </row>
     <row r="6">
@@ -722,7 +722,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9606.ENSP00000263967</t>
+          <t>9606.ENSP00000269305</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PIK3CA</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.947</v>
+        <v>0.887</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -758,16 +758,16 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.128</v>
+        <v>0.076</v>
       </c>
       <c r="L6" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0.931</v>
+        <v>0.883</v>
       </c>
     </row>
     <row r="7">
@@ -776,22 +776,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9606.ENSP00000263967</t>
+          <t>9606.ENSP00000269305</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9606.ENSP00000419060</t>
+          <t>9606.ENSP00000495360</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PIK3CA</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BRAF</t>
+          <t>CTNNB1</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.947</v>
+        <v>0.927</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -812,16 +812,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.128</v>
+        <v>0.049</v>
       </c>
       <c r="L7" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0.931</v>
+        <v>0.927</v>
       </c>
     </row>
     <row r="8">
@@ -830,7 +830,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9606.ENSP00000263967</t>
+          <t>9606.ENSP00000269305</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PIK3CA</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.995</v>
+        <v>0.999</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -866,16 +866,16 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.112</v>
+        <v>0.067</v>
       </c>
       <c r="L8" t="n">
-        <v>0.134</v>
+        <v>0.748</v>
       </c>
       <c r="M8" t="n">
         <v>0.9</v>
       </c>
       <c r="N8" t="n">
-        <v>0.949</v>
+        <v>0.968</v>
       </c>
     </row>
     <row r="9">
@@ -884,22 +884,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9606.ENSP00000263967</t>
+          <t>9606.ENSP00000361021</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9606.ENSP00000361021</t>
+          <t>9606.ENSP00000495360</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PIK3CA</t>
+          <t>PTEN</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>PTEN</t>
+          <t>CTNNB1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0.995</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -920,16 +920,16 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.112</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>0.134</v>
+        <v>0.527</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0.949</v>
+        <v>0.881</v>
       </c>
     </row>
     <row r="10">
@@ -938,7 +938,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9606.ENSP00000269305</t>
+          <t>9606.ENSP00000361021</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>PTEN</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.887</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -974,16 +974,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.076</v>
+        <v>0.094</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.206</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0.883</v>
+        <v>0.927</v>
       </c>
     </row>
     <row r="11">
@@ -992,22 +992,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9606.ENSP00000269305</t>
+          <t>9606.ENSP00000419060</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9606.ENSP00000419060</t>
+          <t>9606.ENSP00000495360</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>BRAF</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BRAF</t>
+          <t>CTNNB1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.887</v>
+        <v>0.795</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1028,555 +1028,15 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.076</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.098</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0.883</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000269305</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>TP53</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>0.927</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.049</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.927</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000269305</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>TP53</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>0.927</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.049</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.927</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000269305</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>TP53</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>0.999</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.748</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.968</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000269305</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>TP53</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>0.999</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.748</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.968</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>0.9429999999999999</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.527</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.881</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>0.9429999999999999</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.527</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.881</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000419060</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>BRAF</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>0.9429999999999999</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.094</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.206</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.927</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000361021</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000419060</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>PTEN</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>BRAF</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>0.9429999999999999</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.094</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.206</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0.927</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000419060</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>BRAF</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.771</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000419060</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>9606.ENSP00000495360</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>BRAF</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CTNNB1</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>9606</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
         <v>0.771</v>
       </c>
     </row>

</xml_diff>